<commit_message>
Test cases for RCC module
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/RCC.xlsx
+++ b/src/test/resources/xls/RCC.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>TCID</t>
   </si>
@@ -30,6 +30,18 @@
   </si>
   <si>
     <t>Results</t>
+  </si>
+  <si>
+    <t>OBT</t>
+  </si>
+  <si>
+    <t>Verifying the invitations</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>RCC010</t>
   </si>
 </sst>
 </file>
@@ -94,11 +106,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -393,10 +406,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -425,6 +438,21 @@
         <v>4</v>
       </c>
     </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="2"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Added new script to RCC
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/RCC.xlsx
+++ b/src/test/resources/xls/RCC.xlsx
@@ -4,18 +4,19 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2580" windowWidth="14595" windowHeight="9795"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="12270" windowHeight="6420"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
     <sheet name="Test Case Steps" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="125725"/>
+  <oleSize ref="A1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
   <si>
     <t>TCID</t>
   </si>
@@ -42,6 +43,15 @@
   </si>
   <si>
     <t>RCC010</t>
+  </si>
+  <si>
+    <t>RCC003</t>
+  </si>
+  <si>
+    <t>ABC</t>
+  </si>
+  <si>
+    <t>Verifying the invitation information</t>
   </si>
 </sst>
 </file>
@@ -406,10 +416,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -453,6 +463,20 @@
       </c>
       <c r="E2" s="2"/>
     </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" t="s">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
RCC new Script implementation
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/RCC.xlsx
+++ b/src/test/resources/xls/RCC.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sb94731\git\Newworspace17oct\src\test\resources\xls\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="2520" windowWidth="12270" windowHeight="6420"/>
   </bookViews>
@@ -20,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="18">
   <si>
     <t>TCID</t>
   </si>
@@ -65,13 +60,22 @@
   </si>
   <si>
     <t>Verifying the groups and invitation count</t>
+  </si>
+  <si>
+    <t>OPQA-3455</t>
+  </si>
+  <si>
+    <t>Verify that user is able to add an article to the group from search results page.</t>
+  </si>
+  <si>
+    <t>RCC111</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -195,7 +199,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -227,10 +231,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -262,7 +265,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -438,14 +440,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="12.85546875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="13.85546875" customWidth="1" collapsed="1"/>
@@ -455,7 +457,7 @@
     <col min="6" max="8" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -472,7 +474,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5">
       <c r="A2" s="2" t="s">
         <v>8</v>
       </c>
@@ -487,33 +489,50 @@
       </c>
       <c r="E2" s="2"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="3" spans="1:5">
+      <c r="A3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="2" t="s">
         <v>7</v>
       </c>
+      <c r="E3" s="2"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="4" spans="1:5">
+      <c r="A4" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="2" t="s">
         <v>7</v>
       </c>
+      <c r="E4" s="2"/>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -522,14 +541,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
New scritps are created in RCC Module.
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/RCC.xlsx
+++ b/src/test/resources/xls/RCC.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2520" windowWidth="12270" windowHeight="6420"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="12276" windowHeight="6420"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="26">
   <si>
     <t>TCID</t>
   </si>
@@ -69,6 +69,30 @@
   </si>
   <si>
     <t>RCC111</t>
+  </si>
+  <si>
+    <t>ABCD1</t>
+  </si>
+  <si>
+    <t>ABCD2</t>
+  </si>
+  <si>
+    <t>ABCD3</t>
+  </si>
+  <si>
+    <t>ABCD4</t>
+  </si>
+  <si>
+    <t>RCC002</t>
+  </si>
+  <si>
+    <t>RCC007</t>
+  </si>
+  <si>
+    <t>RCC008</t>
+  </si>
+  <si>
+    <t>RCC012</t>
   </si>
 </sst>
 </file>
@@ -441,20 +465,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="12.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="13.85546875" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="109.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="9.5703125" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="7.42578125" customWidth="1" collapsed="1"/>
-    <col min="6" max="8" width="9.140625" customWidth="1"/>
+    <col min="1" max="1" width="12.88671875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="13.88671875" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="109.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="9.5546875" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="7.44140625" customWidth="1" collapsed="1"/>
+    <col min="6" max="8" width="9.109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -533,6 +557,66 @@
         <v>7</v>
       </c>
       <c r="E5" s="2"/>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" s="2"/>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E7" s="2"/>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E8" s="2"/>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E9" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -548,7 +632,7 @@
       <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
New scripts are created in RCC Module
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/RCC.xlsx
+++ b/src/test/resources/xls/RCC.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="27">
   <si>
     <t>TCID</t>
   </si>
@@ -93,6 +93,9 @@
   </si>
   <si>
     <t>RCC012</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify that user is able to add an article to the group from search results   page.    </t>
   </si>
 </sst>
 </file>
@@ -467,8 +470,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -611,7 +614,7 @@
         <v>21</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>7</v>

</xml_diff>

<commit_message>
Rcc script is completed
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/RCC.xlsx
+++ b/src/test/resources/xls/RCC.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2520" windowWidth="12276" windowHeight="6420"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="12270" windowHeight="6420"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="30">
   <si>
     <t>TCID</t>
   </si>
@@ -96,6 +96,15 @@
   </si>
   <si>
     <t>Verify that user is able to add an article to the group from search results  page.</t>
+  </si>
+  <si>
+    <t>RCC011</t>
+  </si>
+  <si>
+    <t>OBT2</t>
+  </si>
+  <si>
+    <t>Verify the invitations scenario</t>
   </si>
 </sst>
 </file>
@@ -160,12 +169,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -468,20 +478,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="12.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="13.88671875" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="109.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="9.5546875" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="7.44140625" customWidth="1" collapsed="1"/>
-    <col min="6" max="8" width="9.109375" customWidth="1"/>
+    <col min="1" max="1" width="12.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="13.85546875" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="109.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="9.5703125" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="7.42578125" customWidth="1" collapsed="1"/>
+    <col min="6" max="8" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -620,6 +630,21 @@
         <v>7</v>
       </c>
       <c r="E9" s="2"/>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E10" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -635,7 +660,7 @@
       <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added new Script RCC0001
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/RCC.xlsx
+++ b/src/test/resources/xls/RCC.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="2520" windowWidth="12270" windowHeight="6420"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="31">
   <si>
     <t>TCID</t>
   </si>
@@ -105,13 +105,16 @@
   </si>
   <si>
     <t>Verify the invitations scenario</t>
+  </si>
+  <si>
+    <t>RCC0001</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -142,7 +145,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -165,23 +168,63 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -268,6 +311,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -302,6 +346,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -477,14 +522,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="A13" sqref="A13:XFD13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.85546875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="13.85546875" customWidth="1" collapsed="1"/>
@@ -494,7 +539,7 @@
     <col min="6" max="8" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -511,7 +556,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>8</v>
       </c>
@@ -526,7 +571,7 @@
       </c>
       <c r="E2" s="2"/>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>9</v>
       </c>
@@ -541,7 +586,7 @@
       </c>
       <c r="E3" s="2"/>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>12</v>
       </c>
@@ -556,7 +601,7 @@
       </c>
       <c r="E4" s="2"/>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>17</v>
       </c>
@@ -571,7 +616,7 @@
       </c>
       <c r="E5" s="2"/>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>22</v>
       </c>
@@ -586,7 +631,7 @@
       </c>
       <c r="E6" s="2"/>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>23</v>
       </c>
@@ -601,7 +646,7 @@
       </c>
       <c r="E7" s="2"/>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>24</v>
       </c>
@@ -616,7 +661,7 @@
       </c>
       <c r="E8" s="2"/>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>25</v>
       </c>
@@ -631,7 +676,7 @@
       </c>
       <c r="E9" s="2"/>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>27</v>
       </c>
@@ -645,6 +690,25 @@
         <v>7</v>
       </c>
       <c r="E10" s="2"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>30</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -653,14 +717,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
updated test cases in RCC.xlsx
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/RCC.xlsx
+++ b/src/test/resources/xls/RCC.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="2520" windowWidth="12270" windowHeight="6420"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="32">
   <si>
     <t>TCID</t>
   </si>
@@ -62,9 +62,6 @@
     <t>Verifying the groups and invitation count</t>
   </si>
   <si>
-    <t>OPQA-3455</t>
-  </si>
-  <si>
     <t>Verify that user is able to add an article to the group from search results page.</t>
   </si>
   <si>
@@ -108,13 +105,19 @@
   </si>
   <si>
     <t>RCC0001</t>
+  </si>
+  <si>
+    <t>Verify that user is able to add an article to the group from search results page.||Verify that user is able to add a post to the group from search results page.||Verify that user is able to add a patent to the group from search results page.</t>
+  </si>
+  <si>
+    <t>OPQA-3455||OPQA-3459||OPQA-3463</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -145,7 +148,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -168,29 +171,22 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -311,7 +307,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -346,7 +341,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -522,24 +516,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13:XFD13"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="12.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="13.85546875" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="18.85546875" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="109.42578125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="9.5703125" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="7.42578125" customWidth="1" collapsed="1"/>
     <col min="6" max="8" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -556,7 +550,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5">
       <c r="A2" s="2" t="s">
         <v>8</v>
       </c>
@@ -571,7 +565,7 @@
       </c>
       <c r="E2" s="2"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5">
       <c r="A3" s="2" t="s">
         <v>9</v>
       </c>
@@ -586,7 +580,7 @@
       </c>
       <c r="E3" s="2"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5">
       <c r="A4" s="2" t="s">
         <v>12</v>
       </c>
@@ -601,114 +595,117 @@
       </c>
       <c r="E4" s="2"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="60">
       <c r="A5" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="2"/>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="C6" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E5" s="2"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
+      <c r="D6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" s="2"/>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B7" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C6" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E6" s="2"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
+      <c r="C7" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E7" s="2"/>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B8" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C7" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E7" s="2"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
+      <c r="C8" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E8" s="2"/>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B9" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C8" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E8" s="2"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
+      <c r="C9" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B9" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C9" s="2" t="s">
+      <c r="D9" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E9" s="2"/>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="D9" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E9" s="2"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
+      <c r="B10" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="C10" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="D10" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E10" s="2"/>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" s="2" t="s">
         <v>29</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E10" s="2"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>30</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="4"/>
+        <v>15</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E11" s="2"/>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" s="5"/>
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -717,14 +714,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added new script in RCC Module and modified IAM.xml and LocalRun.xml
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/RCC.xlsx
+++ b/src/test/resources/xls/RCC.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2520" windowWidth="12270" windowHeight="6420"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="12276" windowHeight="6420"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="37">
   <si>
     <t>TCID</t>
   </si>
@@ -120,6 +120,12 @@
   </si>
   <si>
     <t>OPQA-3454||OPQA-3458||OPQA-3462</t>
+  </si>
+  <si>
+    <t>DEF</t>
+  </si>
+  <si>
+    <t>RCC006</t>
   </si>
 </sst>
 </file>
@@ -184,7 +190,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -192,11 +198,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -534,18 +535,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="12.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="18.85546875" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="109.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="9.5703125" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="7.42578125" customWidth="1" collapsed="1"/>
-    <col min="6" max="8" width="9.140625" customWidth="1"/>
+    <col min="1" max="1" width="12.88671875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="18.88671875" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="109.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="9.5546875" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="7.44140625" customWidth="1" collapsed="1"/>
+    <col min="6" max="8" width="9.109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -610,7 +611,7 @@
       </c>
       <c r="E4" s="2"/>
     </row>
-    <row r="5" spans="1:5" ht="30">
+    <row r="5" spans="1:5" ht="28.8">
       <c r="A5" s="2" t="s">
         <v>16</v>
       </c>
@@ -715,14 +716,14 @@
       </c>
       <c r="E11" s="2"/>
     </row>
-    <row r="12" spans="1:5" ht="30">
+    <row r="12" spans="1:5" ht="28.8">
       <c r="A12" s="2" t="s">
         <v>32</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="C12" s="8" t="s">
+      <c r="C12" s="5" t="s">
         <v>33</v>
       </c>
       <c r="D12" s="2" t="s">
@@ -731,11 +732,19 @@
       <c r="E12" s="2"/>
     </row>
     <row r="13" spans="1:5">
-      <c r="A13" s="5"/>
-      <c r="B13" s="5"/>
-      <c r="C13" s="7"/>
-      <c r="D13" s="6"/>
-      <c r="E13" s="5"/>
+      <c r="A13" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E13" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -751,7 +760,7 @@
       <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Test cases is added in RCC module
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/RCC.xlsx
+++ b/src/test/resources/xls/RCC.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2520" windowWidth="12276" windowHeight="6420"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="12270" windowHeight="6420"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="40">
   <si>
     <t>TCID</t>
   </si>
@@ -126,6 +126,15 @@
   </si>
   <si>
     <t>RCC006</t>
+  </si>
+  <si>
+    <t>RCC013</t>
+  </si>
+  <si>
+    <t>OBT3</t>
+  </si>
+  <si>
+    <t>Verifying updated group details in  group detail page and group list page</t>
   </si>
 </sst>
 </file>
@@ -533,20 +542,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="12.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="18.88671875" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="109.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="9.5546875" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="7.44140625" customWidth="1" collapsed="1"/>
-    <col min="6" max="8" width="9.109375" customWidth="1"/>
+    <col min="1" max="1" width="12.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="18.85546875" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="109.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="9.5703125" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="7.42578125" customWidth="1" collapsed="1"/>
+    <col min="6" max="8" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -611,7 +620,7 @@
       </c>
       <c r="E4" s="2"/>
     </row>
-    <row r="5" spans="1:5" ht="28.8">
+    <row r="5" spans="1:5" ht="30">
       <c r="A5" s="2" t="s">
         <v>16</v>
       </c>
@@ -716,7 +725,7 @@
       </c>
       <c r="E11" s="2"/>
     </row>
-    <row r="12" spans="1:5" ht="28.8">
+    <row r="12" spans="1:5" ht="30">
       <c r="A12" s="2" t="s">
         <v>32</v>
       </c>
@@ -745,6 +754,21 @@
         <v>7</v>
       </c>
       <c r="E13" s="2"/>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E14" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -760,7 +784,7 @@
       <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
chages in RCC XLSX
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/RCC.xlsx
+++ b/src/test/resources/xls/RCC.xlsx
@@ -563,7 +563,7 @@
   <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -788,7 +788,7 @@
       </c>
       <c r="E14" s="2"/>
     </row>
-    <row r="15" spans="1:5" ht="45">
+    <row r="15" spans="1:5" ht="34.5" customHeight="1">
       <c r="A15" s="2" t="s">
         <v>40</v>
       </c>

</xml_diff>

<commit_message>
Added new test cases in RCC module
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/RCC.xlsx
+++ b/src/test/resources/xls/RCC.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sb94731\git\Newworspace17oct\src\test\resources\xls\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="2520" windowWidth="12270" windowHeight="6420"/>
   </bookViews>
@@ -20,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="48">
   <si>
     <t>TCID</t>
   </si>
@@ -158,13 +153,19 @@
   </si>
   <si>
     <t>Verifying the Group's cancel and save buttons after creating new group</t>
+  </si>
+  <si>
+    <t>RCC100</t>
+  </si>
+  <si>
+    <t>Verify the sorting options</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -228,7 +229,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -243,6 +244,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -332,7 +336,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -364,10 +368,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -399,7 +402,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -575,14 +577,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E16"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="A17" sqref="A17:E17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="12.85546875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="18.85546875" customWidth="1" collapsed="1"/>
@@ -592,7 +594,7 @@
     <col min="6" max="8" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -609,7 +611,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5">
       <c r="A2" s="2" t="s">
         <v>8</v>
       </c>
@@ -624,7 +626,7 @@
       </c>
       <c r="E2" s="2"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5">
       <c r="A3" s="2" t="s">
         <v>9</v>
       </c>
@@ -639,7 +641,7 @@
       </c>
       <c r="E3" s="2"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5">
       <c r="A4" s="2" t="s">
         <v>12</v>
       </c>
@@ -654,7 +656,7 @@
       </c>
       <c r="E4" s="2"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5">
       <c r="A5" s="2" t="s">
         <v>43</v>
       </c>
@@ -669,7 +671,7 @@
       </c>
       <c r="E5" s="2"/>
     </row>
-    <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="30">
       <c r="A6" s="2" t="s">
         <v>16</v>
       </c>
@@ -684,7 +686,7 @@
       </c>
       <c r="E6" s="2"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5">
       <c r="A7" s="2" t="s">
         <v>21</v>
       </c>
@@ -699,7 +701,7 @@
       </c>
       <c r="E7" s="2"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5">
       <c r="A8" s="2" t="s">
         <v>22</v>
       </c>
@@ -714,7 +716,7 @@
       </c>
       <c r="E8" s="2"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5">
       <c r="A9" s="2" t="s">
         <v>23</v>
       </c>
@@ -729,7 +731,7 @@
       </c>
       <c r="E9" s="2"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5">
       <c r="A10" s="2" t="s">
         <v>24</v>
       </c>
@@ -744,7 +746,7 @@
       </c>
       <c r="E10" s="2"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5">
       <c r="A11" s="3" t="s">
         <v>26</v>
       </c>
@@ -759,7 +761,7 @@
       </c>
       <c r="E11" s="2"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5">
       <c r="A12" s="2" t="s">
         <v>29</v>
       </c>
@@ -774,7 +776,7 @@
       </c>
       <c r="E12" s="2"/>
     </row>
-    <row r="13" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" ht="30">
       <c r="A13" s="2" t="s">
         <v>32</v>
       </c>
@@ -789,7 +791,7 @@
       </c>
       <c r="E13" s="2"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5">
       <c r="A14" s="2" t="s">
         <v>36</v>
       </c>
@@ -804,7 +806,7 @@
       </c>
       <c r="E14" s="2"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5">
       <c r="A15" s="3" t="s">
         <v>37</v>
       </c>
@@ -819,7 +821,7 @@
       </c>
       <c r="E15" s="2"/>
     </row>
-    <row r="16" spans="1:5" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" ht="34.5" customHeight="1">
       <c r="A16" s="2" t="s">
         <v>40</v>
       </c>
@@ -833,6 +835,21 @@
         <v>7</v>
       </c>
       <c r="E16" s="2"/>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E17" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -841,14 +858,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added new Scripts in RCC Module.
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/RCC.xlsx
+++ b/src/test/resources/xls/RCC.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2520" windowWidth="12270" windowHeight="6420"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="12276" windowHeight="6420"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="58">
   <si>
     <t>TCID</t>
   </si>
@@ -186,6 +186,9 @@
   </si>
   <si>
     <t>OPQA-3469||OPQA-3473||OPQA-3477</t>
+  </si>
+  <si>
+    <t>RCC104</t>
   </si>
 </sst>
 </file>
@@ -608,20 +611,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E20"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="12.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="18.85546875" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="109.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="9.5703125" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="7.42578125" customWidth="1" collapsed="1"/>
-    <col min="6" max="8" width="9.140625" customWidth="1"/>
+    <col min="1" max="1" width="12.88671875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="18.88671875" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="109.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="9.5546875" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="7.44140625" customWidth="1" collapsed="1"/>
+    <col min="6" max="8" width="9.109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -701,7 +704,7 @@
       </c>
       <c r="E5" s="2"/>
     </row>
-    <row r="6" spans="1:5" ht="30">
+    <row r="6" spans="1:5" ht="28.8">
       <c r="A6" s="2" t="s">
         <v>16</v>
       </c>
@@ -806,7 +809,7 @@
       </c>
       <c r="E12" s="2"/>
     </row>
-    <row r="13" spans="1:5" ht="30">
+    <row r="13" spans="1:5" ht="28.8">
       <c r="A13" s="2" t="s">
         <v>32</v>
       </c>
@@ -881,7 +884,7 @@
       </c>
       <c r="E17" s="2"/>
     </row>
-    <row r="18" spans="1:5" ht="45">
+    <row r="18" spans="1:5" ht="43.2">
       <c r="A18" s="2" t="s">
         <v>48</v>
       </c>
@@ -896,7 +899,7 @@
       </c>
       <c r="E18" s="2"/>
     </row>
-    <row r="19" spans="1:5" ht="45">
+    <row r="19" spans="1:5" ht="28.8">
       <c r="A19" s="2" t="s">
         <v>51</v>
       </c>
@@ -911,7 +914,7 @@
       </c>
       <c r="E19" s="2"/>
     </row>
-    <row r="20" spans="1:5" ht="45">
+    <row r="20" spans="1:5" ht="43.2">
       <c r="A20" s="2" t="s">
         <v>54</v>
       </c>
@@ -925,6 +928,21 @@
         <v>7</v>
       </c>
       <c r="E20" s="2"/>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E21" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -940,7 +958,7 @@
       <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added New Scripts for RCC and modified ENWIAM54.
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/RCC.xlsx
+++ b/src/test/resources/xls/RCC.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="2520" windowWidth="12270" windowHeight="6420"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="70">
   <si>
     <t>TCID</t>
   </si>
@@ -198,13 +198,40 @@
   </si>
   <si>
     <t>Verify that user is able to add an article to the multiple groups from watch list details page.</t>
+  </si>
+  <si>
+    <t>RCC0002</t>
+  </si>
+  <si>
+    <t>OPQA-1570||OPQA-1576||OPQA-1572</t>
+  </si>
+  <si>
+    <t>1.Verify that group owner is able to edit the group with group name of 2 character and without any description from group details page.2.Verify that during edit group, clicking 'Save' button will close the form and show the updated group details in view mode.3.Verify that group owner is not able to edit the group with blank group name or with 1 character in group name from group details page.</t>
+  </si>
+  <si>
+    <t>RCC0003</t>
+  </si>
+  <si>
+    <t>OPQA-1577||OPQA-1571||OPQA-1573</t>
+  </si>
+  <si>
+    <t>1.Verify that during edit group, clicking 'Cancel' button deletes all modified information and show the group details in view mode.2.Verify that group owner is able to edit the group with group name of 50 characters and without any description from group details page.3.Verify that group owner is not able to edit the group with morethan 50 characters in group name from group details page.</t>
+  </si>
+  <si>
+    <t>RCC0004</t>
+  </si>
+  <si>
+    <t>OPQA-1578||OPQA-1579</t>
+  </si>
+  <si>
+    <t>1.Verify that group owner is able to edit group description with &lt;= 500 characters from group details page.2Verify that group owner is not able to edit group description with more than 500 characters from group details page.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -268,7 +295,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -289,6 +316,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -410,6 +440,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -444,6 +475,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -619,24 +651,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E22"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23:E25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="18.85546875" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="22.5703125" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="109.42578125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="9.5703125" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="7.42578125" customWidth="1" collapsed="1"/>
     <col min="6" max="8" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -653,7 +685,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>8</v>
       </c>
@@ -668,7 +700,7 @@
       </c>
       <c r="E2" s="2"/>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>9</v>
       </c>
@@ -683,7 +715,7 @@
       </c>
       <c r="E3" s="2"/>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>12</v>
       </c>
@@ -698,7 +730,7 @@
       </c>
       <c r="E4" s="2"/>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>43</v>
       </c>
@@ -713,7 +745,7 @@
       </c>
       <c r="E5" s="2"/>
     </row>
-    <row r="6" spans="1:5" ht="30">
+    <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>16</v>
       </c>
@@ -728,7 +760,7 @@
       </c>
       <c r="E6" s="2"/>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>21</v>
       </c>
@@ -743,7 +775,7 @@
       </c>
       <c r="E7" s="2"/>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>22</v>
       </c>
@@ -758,7 +790,7 @@
       </c>
       <c r="E8" s="2"/>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>23</v>
       </c>
@@ -773,7 +805,7 @@
       </c>
       <c r="E9" s="2"/>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>24</v>
       </c>
@@ -788,7 +820,7 @@
       </c>
       <c r="E10" s="2"/>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>26</v>
       </c>
@@ -803,7 +835,7 @@
       </c>
       <c r="E11" s="2"/>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>29</v>
       </c>
@@ -818,7 +850,7 @@
       </c>
       <c r="E12" s="2"/>
     </row>
-    <row r="13" spans="1:5" ht="30">
+    <row r="13" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>32</v>
       </c>
@@ -833,7 +865,7 @@
       </c>
       <c r="E13" s="2"/>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>36</v>
       </c>
@@ -848,7 +880,7 @@
       </c>
       <c r="E14" s="2"/>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>37</v>
       </c>
@@ -863,7 +895,7 @@
       </c>
       <c r="E15" s="2"/>
     </row>
-    <row r="16" spans="1:5" ht="34.5" customHeight="1">
+    <row r="16" spans="1:5" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>40</v>
       </c>
@@ -878,7 +910,7 @@
       </c>
       <c r="E16" s="2"/>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>46</v>
       </c>
@@ -893,11 +925,11 @@
       </c>
       <c r="E17" s="2"/>
     </row>
-    <row r="18" spans="1:5" ht="45">
+    <row r="18" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="B18" s="4" t="s">
+      <c r="B18" s="9" t="s">
         <v>50</v>
       </c>
       <c r="C18" s="6" t="s">
@@ -908,7 +940,7 @@
       </c>
       <c r="E18" s="2"/>
     </row>
-    <row r="19" spans="1:5" ht="45">
+    <row r="19" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>51</v>
       </c>
@@ -923,7 +955,7 @@
       </c>
       <c r="E19" s="2"/>
     </row>
-    <row r="20" spans="1:5" ht="45">
+    <row r="20" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>54</v>
       </c>
@@ -938,7 +970,7 @@
       </c>
       <c r="E20" s="2"/>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>57</v>
       </c>
@@ -953,7 +985,7 @@
       </c>
       <c r="E21" s="2"/>
     </row>
-    <row r="22" spans="1:5">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>58</v>
       </c>
@@ -967,6 +999,51 @@
         <v>7</v>
       </c>
       <c r="E22" s="2"/>
+    </row>
+    <row r="23" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B23" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E23" s="2"/>
+    </row>
+    <row r="24" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B24" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E24" s="2"/>
+    </row>
+    <row r="25" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B25" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E25" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -975,14 +1052,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
MOdified test case in RCC module
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/RCC.xlsx
+++ b/src/test/resources/xls/RCC.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="2520" windowWidth="12270" windowHeight="6420"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="72">
   <si>
     <t>TCID</t>
   </si>
@@ -225,13 +225,19 @@
   </si>
   <si>
     <t>1.Verify that group owner is able to edit group description with &lt;= 500 characters from group details page.2Verify that group owner is not able to edit group description with more than 500 characters from group details page.</t>
+  </si>
+  <si>
+    <t>RCC101</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify sort by most recent activity </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -295,7 +301,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -318,6 +324,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -440,7 +449,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -475,7 +483,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -651,14 +658,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E25"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E26"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23:E25"/>
+      <selection activeCell="A26" sqref="A26:E26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="12.85546875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="22.5703125" customWidth="1" collapsed="1"/>
@@ -668,7 +675,7 @@
     <col min="6" max="8" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -685,7 +692,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5">
       <c r="A2" s="2" t="s">
         <v>8</v>
       </c>
@@ -700,7 +707,7 @@
       </c>
       <c r="E2" s="2"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5">
       <c r="A3" s="2" t="s">
         <v>9</v>
       </c>
@@ -715,7 +722,7 @@
       </c>
       <c r="E3" s="2"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5">
       <c r="A4" s="2" t="s">
         <v>12</v>
       </c>
@@ -730,7 +737,7 @@
       </c>
       <c r="E4" s="2"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5">
       <c r="A5" s="2" t="s">
         <v>43</v>
       </c>
@@ -745,7 +752,7 @@
       </c>
       <c r="E5" s="2"/>
     </row>
-    <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="30">
       <c r="A6" s="2" t="s">
         <v>16</v>
       </c>
@@ -760,7 +767,7 @@
       </c>
       <c r="E6" s="2"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5">
       <c r="A7" s="2" t="s">
         <v>21</v>
       </c>
@@ -775,7 +782,7 @@
       </c>
       <c r="E7" s="2"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5">
       <c r="A8" s="2" t="s">
         <v>22</v>
       </c>
@@ -790,7 +797,7 @@
       </c>
       <c r="E8" s="2"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5">
       <c r="A9" s="2" t="s">
         <v>23</v>
       </c>
@@ -805,7 +812,7 @@
       </c>
       <c r="E9" s="2"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5">
       <c r="A10" s="2" t="s">
         <v>24</v>
       </c>
@@ -820,7 +827,7 @@
       </c>
       <c r="E10" s="2"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5">
       <c r="A11" s="3" t="s">
         <v>26</v>
       </c>
@@ -835,7 +842,7 @@
       </c>
       <c r="E11" s="2"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5">
       <c r="A12" s="2" t="s">
         <v>29</v>
       </c>
@@ -850,7 +857,7 @@
       </c>
       <c r="E12" s="2"/>
     </row>
-    <row r="13" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" ht="30">
       <c r="A13" s="2" t="s">
         <v>32</v>
       </c>
@@ -865,7 +872,7 @@
       </c>
       <c r="E13" s="2"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5">
       <c r="A14" s="2" t="s">
         <v>36</v>
       </c>
@@ -880,7 +887,7 @@
       </c>
       <c r="E14" s="2"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5">
       <c r="A15" s="3" t="s">
         <v>37</v>
       </c>
@@ -895,7 +902,7 @@
       </c>
       <c r="E15" s="2"/>
     </row>
-    <row r="16" spans="1:5" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" ht="34.5" customHeight="1">
       <c r="A16" s="2" t="s">
         <v>40</v>
       </c>
@@ -910,7 +917,7 @@
       </c>
       <c r="E16" s="2"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5">
       <c r="A17" s="3" t="s">
         <v>46</v>
       </c>
@@ -925,7 +932,7 @@
       </c>
       <c r="E17" s="2"/>
     </row>
-    <row r="18" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" ht="45">
       <c r="A18" s="2" t="s">
         <v>48</v>
       </c>
@@ -940,7 +947,7 @@
       </c>
       <c r="E18" s="2"/>
     </row>
-    <row r="19" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" ht="45">
       <c r="A19" s="2" t="s">
         <v>51</v>
       </c>
@@ -955,7 +962,7 @@
       </c>
       <c r="E19" s="2"/>
     </row>
-    <row r="20" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" ht="45">
       <c r="A20" s="2" t="s">
         <v>54</v>
       </c>
@@ -970,7 +977,7 @@
       </c>
       <c r="E20" s="2"/>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5">
       <c r="A21" s="2" t="s">
         <v>57</v>
       </c>
@@ -985,7 +992,7 @@
       </c>
       <c r="E21" s="2"/>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5">
       <c r="A22" s="2" t="s">
         <v>58</v>
       </c>
@@ -1000,7 +1007,7 @@
       </c>
       <c r="E22" s="2"/>
     </row>
-    <row r="23" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" ht="60">
       <c r="A23" s="2" t="s">
         <v>61</v>
       </c>
@@ -1015,7 +1022,7 @@
       </c>
       <c r="E23" s="2"/>
     </row>
-    <row r="24" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" ht="60">
       <c r="A24" s="2" t="s">
         <v>64</v>
       </c>
@@ -1030,7 +1037,7 @@
       </c>
       <c r="E24" s="2"/>
     </row>
-    <row r="25" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" ht="30">
       <c r="A25" s="2" t="s">
         <v>67</v>
       </c>
@@ -1044,6 +1051,21 @@
         <v>7</v>
       </c>
       <c r="E25" s="2"/>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="B26" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="C26" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E26" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1052,14 +1074,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
New Scripts for RCC( RCC090,RCC091,RCC092)
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/RCC.xlsx
+++ b/src/test/resources/xls/RCC.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="2520" windowWidth="12270" windowHeight="6420"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="81">
   <si>
     <t>TCID</t>
   </si>
@@ -231,13 +231,40 @@
   </si>
   <si>
     <t xml:space="preserve">Verify sort by most recent activity </t>
+  </si>
+  <si>
+    <t>RCC090</t>
+  </si>
+  <si>
+    <t>OPQA-1467||OPQA-1518</t>
+  </si>
+  <si>
+    <t>Verify that Group owner user is able to add cover photo to a group || Verify that cover photo is displayed properly from groups tab for the newly created group.</t>
+  </si>
+  <si>
+    <t>RCC091</t>
+  </si>
+  <si>
+    <t>OPQA-1581</t>
+  </si>
+  <si>
+    <t>Verify that group owner is able to modify the cover photo of the group through Edit option from group details page.</t>
+  </si>
+  <si>
+    <t>RCC092</t>
+  </si>
+  <si>
+    <t>OPQA-1584</t>
+  </si>
+  <si>
+    <t>Verify that group owner sees option to add an image if cover photo not exists for the group from group details page.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -449,6 +476,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -483,6 +511,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -658,14 +687,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E26"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26:E26"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.85546875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="22.5703125" customWidth="1" collapsed="1"/>
@@ -675,7 +704,7 @@
     <col min="6" max="8" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -692,7 +721,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>8</v>
       </c>
@@ -707,7 +736,7 @@
       </c>
       <c r="E2" s="2"/>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>9</v>
       </c>
@@ -722,7 +751,7 @@
       </c>
       <c r="E3" s="2"/>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>12</v>
       </c>
@@ -737,7 +766,7 @@
       </c>
       <c r="E4" s="2"/>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>43</v>
       </c>
@@ -752,7 +781,7 @@
       </c>
       <c r="E5" s="2"/>
     </row>
-    <row r="6" spans="1:5" ht="30">
+    <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>16</v>
       </c>
@@ -767,7 +796,7 @@
       </c>
       <c r="E6" s="2"/>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>21</v>
       </c>
@@ -782,7 +811,7 @@
       </c>
       <c r="E7" s="2"/>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>22</v>
       </c>
@@ -797,7 +826,7 @@
       </c>
       <c r="E8" s="2"/>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>23</v>
       </c>
@@ -812,7 +841,7 @@
       </c>
       <c r="E9" s="2"/>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>24</v>
       </c>
@@ -827,7 +856,7 @@
       </c>
       <c r="E10" s="2"/>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>26</v>
       </c>
@@ -842,7 +871,7 @@
       </c>
       <c r="E11" s="2"/>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>29</v>
       </c>
@@ -857,7 +886,7 @@
       </c>
       <c r="E12" s="2"/>
     </row>
-    <row r="13" spans="1:5" ht="30">
+    <row r="13" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>32</v>
       </c>
@@ -872,7 +901,7 @@
       </c>
       <c r="E13" s="2"/>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>36</v>
       </c>
@@ -887,7 +916,7 @@
       </c>
       <c r="E14" s="2"/>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>37</v>
       </c>
@@ -902,7 +931,7 @@
       </c>
       <c r="E15" s="2"/>
     </row>
-    <row r="16" spans="1:5" ht="34.5" customHeight="1">
+    <row r="16" spans="1:5" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>40</v>
       </c>
@@ -917,7 +946,7 @@
       </c>
       <c r="E16" s="2"/>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>46</v>
       </c>
@@ -932,7 +961,7 @@
       </c>
       <c r="E17" s="2"/>
     </row>
-    <row r="18" spans="1:5" ht="45">
+    <row r="18" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>48</v>
       </c>
@@ -947,7 +976,7 @@
       </c>
       <c r="E18" s="2"/>
     </row>
-    <row r="19" spans="1:5" ht="45">
+    <row r="19" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>51</v>
       </c>
@@ -962,7 +991,7 @@
       </c>
       <c r="E19" s="2"/>
     </row>
-    <row r="20" spans="1:5" ht="45">
+    <row r="20" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>54</v>
       </c>
@@ -977,7 +1006,7 @@
       </c>
       <c r="E20" s="2"/>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>57</v>
       </c>
@@ -992,7 +1021,7 @@
       </c>
       <c r="E21" s="2"/>
     </row>
-    <row r="22" spans="1:5">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>58</v>
       </c>
@@ -1007,7 +1036,7 @@
       </c>
       <c r="E22" s="2"/>
     </row>
-    <row r="23" spans="1:5" ht="60">
+    <row r="23" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>61</v>
       </c>
@@ -1022,7 +1051,7 @@
       </c>
       <c r="E23" s="2"/>
     </row>
-    <row r="24" spans="1:5" ht="60">
+    <row r="24" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>64</v>
       </c>
@@ -1037,7 +1066,7 @@
       </c>
       <c r="E24" s="2"/>
     </row>
-    <row r="25" spans="1:5" ht="30">
+    <row r="25" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>67</v>
       </c>
@@ -1052,7 +1081,7 @@
       </c>
       <c r="E25" s="2"/>
     </row>
-    <row r="26" spans="1:5">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>70</v>
       </c>
@@ -1066,6 +1095,51 @@
         <v>7</v>
       </c>
       <c r="E26" s="2"/>
+    </row>
+    <row r="27" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B27" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E27" s="2"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="B28" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E28" s="2"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="B29" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="C29" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E29" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1074,14 +1148,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated the scripts with users.
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/RCC.xlsx
+++ b/src/test/resources/xls/RCC.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="2520" windowWidth="12270" windowHeight="6420"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="94">
   <si>
     <t>TCID</t>
   </si>
@@ -258,13 +258,52 @@
   </si>
   <si>
     <t>Verify that group owner sees option to add an image if cover photo not exists for the group from group details page.</t>
+  </si>
+  <si>
+    <t>RCC001</t>
+  </si>
+  <si>
+    <t>TBD</t>
+  </si>
+  <si>
+    <t>RCC009</t>
+  </si>
+  <si>
+    <t>RCC014</t>
+  </si>
+  <si>
+    <t>RCC015</t>
+  </si>
+  <si>
+    <t>RCC016</t>
+  </si>
+  <si>
+    <t>RCC017</t>
+  </si>
+  <si>
+    <t>RCC018</t>
+  </si>
+  <si>
+    <t>RCC019</t>
+  </si>
+  <si>
+    <t>RCC021</t>
+  </si>
+  <si>
+    <t>RCC022</t>
+  </si>
+  <si>
+    <t>RCC023</t>
+  </si>
+  <si>
+    <t>RCC024</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -476,7 +515,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -511,7 +549,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -687,14 +724,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E29"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="12.85546875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="22.5703125" customWidth="1" collapsed="1"/>
@@ -704,7 +741,7 @@
     <col min="6" max="8" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -721,7 +758,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5">
       <c r="A2" s="2" t="s">
         <v>8</v>
       </c>
@@ -736,7 +773,7 @@
       </c>
       <c r="E2" s="2"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5">
       <c r="A3" s="2" t="s">
         <v>9</v>
       </c>
@@ -751,7 +788,7 @@
       </c>
       <c r="E3" s="2"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5">
       <c r="A4" s="2" t="s">
         <v>12</v>
       </c>
@@ -766,7 +803,7 @@
       </c>
       <c r="E4" s="2"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5">
       <c r="A5" s="2" t="s">
         <v>43</v>
       </c>
@@ -781,7 +818,7 @@
       </c>
       <c r="E5" s="2"/>
     </row>
-    <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="30">
       <c r="A6" s="2" t="s">
         <v>16</v>
       </c>
@@ -796,7 +833,7 @@
       </c>
       <c r="E6" s="2"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5">
       <c r="A7" s="2" t="s">
         <v>21</v>
       </c>
@@ -811,7 +848,7 @@
       </c>
       <c r="E7" s="2"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5">
       <c r="A8" s="2" t="s">
         <v>22</v>
       </c>
@@ -826,7 +863,7 @@
       </c>
       <c r="E8" s="2"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5">
       <c r="A9" s="2" t="s">
         <v>23</v>
       </c>
@@ -841,7 +878,7 @@
       </c>
       <c r="E9" s="2"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5">
       <c r="A10" s="2" t="s">
         <v>24</v>
       </c>
@@ -856,7 +893,7 @@
       </c>
       <c r="E10" s="2"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5">
       <c r="A11" s="3" t="s">
         <v>26</v>
       </c>
@@ -871,7 +908,7 @@
       </c>
       <c r="E11" s="2"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5">
       <c r="A12" s="2" t="s">
         <v>29</v>
       </c>
@@ -886,7 +923,7 @@
       </c>
       <c r="E12" s="2"/>
     </row>
-    <row r="13" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" ht="30">
       <c r="A13" s="2" t="s">
         <v>32</v>
       </c>
@@ -901,7 +938,7 @@
       </c>
       <c r="E13" s="2"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5">
       <c r="A14" s="2" t="s">
         <v>36</v>
       </c>
@@ -916,7 +953,7 @@
       </c>
       <c r="E14" s="2"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5">
       <c r="A15" s="3" t="s">
         <v>37</v>
       </c>
@@ -931,7 +968,7 @@
       </c>
       <c r="E15" s="2"/>
     </row>
-    <row r="16" spans="1:5" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" ht="34.5" customHeight="1">
       <c r="A16" s="2" t="s">
         <v>40</v>
       </c>
@@ -946,7 +983,7 @@
       </c>
       <c r="E16" s="2"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5">
       <c r="A17" s="3" t="s">
         <v>46</v>
       </c>
@@ -961,7 +998,7 @@
       </c>
       <c r="E17" s="2"/>
     </row>
-    <row r="18" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" ht="45">
       <c r="A18" s="2" t="s">
         <v>48</v>
       </c>
@@ -976,7 +1013,7 @@
       </c>
       <c r="E18" s="2"/>
     </row>
-    <row r="19" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" ht="45">
       <c r="A19" s="2" t="s">
         <v>51</v>
       </c>
@@ -991,7 +1028,7 @@
       </c>
       <c r="E19" s="2"/>
     </row>
-    <row r="20" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" ht="45">
       <c r="A20" s="2" t="s">
         <v>54</v>
       </c>
@@ -1006,7 +1043,7 @@
       </c>
       <c r="E20" s="2"/>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5">
       <c r="A21" s="2" t="s">
         <v>57</v>
       </c>
@@ -1021,7 +1058,7 @@
       </c>
       <c r="E21" s="2"/>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5">
       <c r="A22" s="2" t="s">
         <v>58</v>
       </c>
@@ -1036,7 +1073,7 @@
       </c>
       <c r="E22" s="2"/>
     </row>
-    <row r="23" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" ht="60">
       <c r="A23" s="2" t="s">
         <v>61</v>
       </c>
@@ -1051,7 +1088,7 @@
       </c>
       <c r="E23" s="2"/>
     </row>
-    <row r="24" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" ht="60">
       <c r="A24" s="2" t="s">
         <v>64</v>
       </c>
@@ -1066,7 +1103,7 @@
       </c>
       <c r="E24" s="2"/>
     </row>
-    <row r="25" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" ht="30">
       <c r="A25" s="2" t="s">
         <v>67</v>
       </c>
@@ -1081,7 +1118,7 @@
       </c>
       <c r="E25" s="2"/>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5">
       <c r="A26" s="3" t="s">
         <v>70</v>
       </c>
@@ -1096,7 +1133,7 @@
       </c>
       <c r="E26" s="2"/>
     </row>
-    <row r="27" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" ht="30">
       <c r="A27" s="2" t="s">
         <v>72</v>
       </c>
@@ -1111,7 +1148,7 @@
       </c>
       <c r="E27" s="2"/>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5">
       <c r="A28" s="2" t="s">
         <v>75</v>
       </c>
@@ -1126,7 +1163,7 @@
       </c>
       <c r="E28" s="2"/>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5">
       <c r="A29" s="3" t="s">
         <v>78</v>
       </c>
@@ -1140,6 +1177,201 @@
         <v>7</v>
       </c>
       <c r="E29" s="2"/>
+    </row>
+    <row r="30" spans="1:5">
+      <c r="A30" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E30" s="2"/>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="A31" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E31" s="2"/>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="A32" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E32" s="2"/>
+    </row>
+    <row r="33" spans="1:5">
+      <c r="A33" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E33" s="2"/>
+    </row>
+    <row r="34" spans="1:5">
+      <c r="A34" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E34" s="2"/>
+    </row>
+    <row r="35" spans="1:5">
+      <c r="A35" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E35" s="2"/>
+    </row>
+    <row r="36" spans="1:5">
+      <c r="A36" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E36" s="2"/>
+    </row>
+    <row r="37" spans="1:5">
+      <c r="A37" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E37" s="2"/>
+    </row>
+    <row r="38" spans="1:5">
+      <c r="A38" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E38" s="2"/>
+    </row>
+    <row r="39" spans="1:5">
+      <c r="A39" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E39" s="2"/>
+    </row>
+    <row r="40" spans="1:5">
+      <c r="A40" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E40" s="2"/>
+    </row>
+    <row r="41" spans="1:5">
+      <c r="A41" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E41" s="2"/>
+    </row>
+    <row r="42" spans="1:5">
+      <c r="A42" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E42" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1148,14 +1380,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
RCC updated the excel
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/RCC.xlsx
+++ b/src/test/resources/xls/RCC.xlsx
@@ -257,9 +257,6 @@
     <t>OPQA-1570||OPQA-1576||OPQA-1572||OPQA-1574</t>
   </si>
   <si>
-    <t>OPQA-1448||OPQA-1451||OPQA-1454||OPQA-1464||OPQA-1465||OPQA-1462</t>
-  </si>
-  <si>
     <t>OPQA-3406||OPQA-3408||OPQA-3411||OPQA-3412||OPQA-3413||OPQA-3414</t>
   </si>
   <si>
@@ -278,9 +275,6 @@
     <t>OPQA-3375</t>
   </si>
   <si>
-    <t>OPQA-1532||OPQA-1550OPQA-1550||OPQA-3365||OPQA-3366||OPQA-1494</t>
-  </si>
-  <si>
     <t>OPQA-1484||OPQA-1486||OPQA-3400||OPQA-1468||OPQA-1590||OPQA-1460</t>
   </si>
   <si>
@@ -347,21 +341,9 @@
     <t>OPQA-3426||OPQA-3437||OPQA-3449</t>
   </si>
   <si>
-    <t>OPQA-1566||OPQA-3451||OPQA-3468</t>
-  </si>
-  <si>
-    <t>OPQA-1529||OPQA-3445||OPQA-3446||OPQA-3447||OPQA-1564||OPQA-3450||OPQA-1565</t>
-  </si>
-  <si>
-    <t>OPQA-1556||OPQA-3438||OPQA-1557||OPQA-1527||OPQA-3442||OPQA-3443||OPQA-3444||OPQA-1551||OPQA-1552</t>
-  </si>
-  <si>
     <t>OPQA-1548||OPQA-1549||OPQA-3428||OPQA-3429||OPQA-3430</t>
   </si>
   <si>
-    <t>OPQA-1534||OPQA-1544||OPQA-1546||OPQA-3427||OPQA-1526||OPQA-3433||OPQA-3434||OPQA-3435</t>
-  </si>
-  <si>
     <t>OPQA-1524||OPQA-3420||OPQA-3421||OPQA-3422||OPQA-1531||OPQA-1533||OPQA-1535||OPQA-1537||OPQA-3423</t>
   </si>
   <si>
@@ -419,10 +401,28 @@
     <t>OPQA-1485||OPQA-3398||OPQA-3369||OPQA-1523||OPQA-1491||OPQA-3380||OPQA-3376</t>
   </si>
   <si>
-    <t>OPQA-3455||OPQA-3459||OPQA-3463||OPQA-1479</t>
-  </si>
-  <si>
     <t>Validate add to group drop down on removing the records from group</t>
+  </si>
+  <si>
+    <t>OPQA-1534||OPQA-1544||OPQA-1546||OPQA-3427||OPQA-1526||OPQA-3433||OPQA-3434||OPQA-3435||OPQA-1507</t>
+  </si>
+  <si>
+    <t>OPQA-1556||OPQA-3438||OPQA-1557||OPQA-1527||OPQA-3442||OPQA-3443||OPQA-3444||OPQA-1551||OPQA-1552||OPQA-1511</t>
+  </si>
+  <si>
+    <t>OPQA-1529||OPQA-3445||OPQA-3446||OPQA-3447||OPQA-1564||OPQA-3450||OPQA-1565||OPQA-1513</t>
+  </si>
+  <si>
+    <t>OPQA-3455||OPQA-3459||OPQA-3463||OPQA-1479||OPQA-1470</t>
+  </si>
+  <si>
+    <t>OPQA-1448||OPQA-1451||OPQA-1454||OPQA-1464||OPQA-1465||OPQA-1462||OPQA-1457||OPQA-1459</t>
+  </si>
+  <si>
+    <t>OPQA-1566||OPQA-3451||OPQA-1568</t>
+  </si>
+  <si>
+    <t>OPQA-1532||OPQA-1550||OPQA-3365||OPQA-3366||OPQA-1494</t>
   </si>
 </sst>
 </file>
@@ -853,14 +853,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="C42" sqref="C42"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="12.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="22.5703125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="50" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="109.42578125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="9.5703125" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="7.42578125" customWidth="1" collapsed="1"/>
@@ -889,10 +889,10 @@
         <v>6</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>81</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>82</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>5</v>
@@ -904,10 +904,10 @@
         <v>7</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>5</v>
@@ -919,7 +919,7 @@
         <v>8</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>87</v>
+        <v>135</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>9</v>
@@ -934,7 +934,7 @@
         <v>29</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>30</v>
@@ -944,12 +944,12 @@
       </c>
       <c r="E5" s="2"/>
     </row>
-    <row r="6" spans="1:5" ht="45">
+    <row r="6" spans="1:5" ht="60">
       <c r="A6" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>19</v>
@@ -964,7 +964,7 @@
         <v>12</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>10</v>
@@ -979,7 +979,7 @@
         <v>13</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>10</v>
@@ -994,7 +994,7 @@
         <v>14</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>10</v>
@@ -1009,7 +1009,7 @@
         <v>15</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>16</v>
@@ -1024,10 +1024,10 @@
         <v>17</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>5</v>
@@ -1039,10 +1039,10 @@
         <v>18</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>80</v>
+        <v>133</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>5</v>
@@ -1069,10 +1069,10 @@
         <v>23</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>5</v>
@@ -1084,7 +1084,7 @@
         <v>24</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>25</v>
@@ -1114,10 +1114,10 @@
         <v>31</v>
       </c>
       <c r="B17" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="C17" s="3" t="s">
         <v>84</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>85</v>
       </c>
       <c r="D17" s="3" t="s">
         <v>5</v>
@@ -1174,10 +1174,10 @@
         <v>41</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D21" s="2" t="s">
         <v>5</v>
@@ -1249,7 +1249,7 @@
         <v>51</v>
       </c>
       <c r="B26" s="10" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C26" s="7" t="s">
         <v>52</v>
@@ -1309,10 +1309,10 @@
         <v>62</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="D30" s="2" t="s">
         <v>5</v>
@@ -1324,10 +1324,10 @@
         <v>63</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D31" s="2" t="s">
         <v>5</v>
@@ -1339,10 +1339,10 @@
         <v>64</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="D32" s="2" t="s">
         <v>5</v>
@@ -1354,10 +1354,10 @@
         <v>65</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D33" s="2" t="s">
         <v>5</v>
@@ -1369,10 +1369,10 @@
         <v>66</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="D34" s="2" t="s">
         <v>5</v>
@@ -1384,10 +1384,10 @@
         <v>67</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>110</v>
+        <v>134</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="D35" s="2" t="s">
         <v>5</v>
@@ -1399,10 +1399,10 @@
         <v>68</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="D36" s="2" t="s">
         <v>5</v>
@@ -1414,10 +1414,10 @@
         <v>69</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="D37" s="2" t="s">
         <v>5</v>
@@ -1429,10 +1429,10 @@
         <v>70</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>114</v>
+        <v>129</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="D38" s="2" t="s">
         <v>5</v>
@@ -1444,10 +1444,10 @@
         <v>71</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>112</v>
+        <v>130</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="D39" s="2" t="s">
         <v>5</v>
@@ -1459,10 +1459,10 @@
         <v>72</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>111</v>
+        <v>131</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="D40" s="2" t="s">
         <v>5</v>
@@ -1474,10 +1474,10 @@
         <v>73</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="D41" s="2" t="s">
         <v>5</v>
@@ -1501,13 +1501,13 @@
     </row>
     <row r="43" spans="1:5">
       <c r="A43" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="B43" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="B43" s="2" t="s">
-        <v>94</v>
-      </c>
       <c r="C43" s="2" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D43" s="2" t="s">
         <v>5</v>
@@ -1516,13 +1516,13 @@
     </row>
     <row r="44" spans="1:5">
       <c r="A44" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="B44" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="B44" s="2" t="s">
-        <v>97</v>
-      </c>
       <c r="C44" s="2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D44" s="2" t="s">
         <v>5</v>
@@ -1531,13 +1531,13 @@
     </row>
     <row r="45" spans="1:5">
       <c r="A45" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="B45" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="B45" s="2" t="s">
-        <v>109</v>
-      </c>
       <c r="C45" s="2" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="D45" s="2" t="s">
         <v>5</v>

</xml_diff>

<commit_message>
added new scripts in RCC119
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/RCC.xlsx
+++ b/src/test/resources/xls/RCC.xlsx
@@ -4,18 +4,19 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2520" windowWidth="12270" windowHeight="6420"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="13395" windowHeight="5820"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
     <sheet name="Test Case Steps" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="125725"/>
+  <oleSize ref="A1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="139">
   <si>
     <t>TCID</t>
   </si>
@@ -423,13 +424,22 @@
   </si>
   <si>
     <t>OPQA-1532||OPQA-1550||OPQA-3365||OPQA-3366||OPQA-1494</t>
+  </si>
+  <si>
+    <t>OPQA-4684</t>
+  </si>
+  <si>
+    <t>Verify the 'Accept Invitation' Link in Invitation email is redirecting to the Particular Group Invitation page</t>
+  </si>
+  <si>
+    <t>RCC119</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -444,6 +454,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF333333"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -466,7 +482,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -489,11 +505,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -521,6 +548,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -851,10 +880,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E45"/>
+  <dimension ref="A1:E47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="B47" sqref="B47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -944,7 +973,7 @@
       </c>
       <c r="E5" s="2"/>
     </row>
-    <row r="6" spans="1:5" ht="60">
+    <row r="6" spans="1:5" ht="30">
       <c r="A6" s="2" t="s">
         <v>11</v>
       </c>
@@ -1064,7 +1093,7 @@
       </c>
       <c r="E13" s="2"/>
     </row>
-    <row r="14" spans="1:5" ht="165">
+    <row r="14" spans="1:5" ht="60">
       <c r="A14" s="2" t="s">
         <v>23</v>
       </c>
@@ -1109,7 +1138,7 @@
       </c>
       <c r="E16" s="2"/>
     </row>
-    <row r="17" spans="1:5" ht="30">
+    <row r="17" spans="1:5">
       <c r="A17" s="3" t="s">
         <v>31</v>
       </c>
@@ -1543,6 +1572,25 @@
         <v>5</v>
       </c>
       <c r="E45" s="2"/>
+    </row>
+    <row r="46" spans="1:5">
+      <c r="A46" s="11" t="s">
+        <v>138</v>
+      </c>
+      <c r="B46" t="s">
+        <v>136</v>
+      </c>
+      <c r="C46" s="12" t="s">
+        <v>137</v>
+      </c>
+      <c r="D46" s="11" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5">
+      <c r="D47" s="11" t="s">
+        <v>5</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>